<commit_message>
modified to fit units.csv
</commit_message>
<xml_diff>
--- a/sample_db/Chem_Eng_Maj.xlsx
+++ b/sample_db/Chem_Eng_Maj.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\racin\Documents\University Stuff\Year 4 Semester 2\CITS3200 Professional Computing\Project\CITS3200Project_Main\sample_db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f15136bb4a599a09/Desktop/UWA/UWA Sem 2 2023/professional computing/CITS3200Project/sample_db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83406E9D-D9B1-4CBF-9796-1D6AC5119EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{83406E9D-D9B1-4CBF-9796-1D6AC5119EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6F2FBED-4F55-4D5A-A3FD-BB84442A7120}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{37AF2BA7-84C2-43E4-9A3A-F3D37D7A3C67}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{37AF2BA7-84C2-43E4-9A3A-F3D37D7A3C67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="104">
   <si>
     <t>unitcode</t>
   </si>
@@ -59,9 +59,6 @@
     <t>credit_points</t>
   </si>
   <si>
-    <t>point_type</t>
-  </si>
-  <si>
     <t>points_req</t>
   </si>
   <si>
@@ -173,15 +170,9 @@
     <t>GENG5507</t>
   </si>
   <si>
-    <t>CORE</t>
-  </si>
-  <si>
     <t>CHPR4408</t>
   </si>
   <si>
-    <t>GROUP_A</t>
-  </si>
-  <si>
     <t>CHPR5520</t>
   </si>
   <si>
@@ -197,9 +188,6 @@
     <t>CITS4009</t>
   </si>
   <si>
-    <t>GROUP_B</t>
-  </si>
-  <si>
     <t>ENVE4401</t>
   </si>
   <si>
@@ -279,6 +267,87 @@
   </si>
   <si>
     <t>CHPR4403</t>
+  </si>
+  <si>
+    <t>Chemistry - Properties and Energetics</t>
+  </si>
+  <si>
+    <t>Chemistry - Structure and Reactivity</t>
+  </si>
+  <si>
+    <t>Mass and Energy Balances</t>
+  </si>
+  <si>
+    <t>Chemical Engineering Thermodynamics</t>
+  </si>
+  <si>
+    <t>Heat and Mass Transfer</t>
+  </si>
+  <si>
+    <t>Process Synthesis and Design 1</t>
+  </si>
+  <si>
+    <t>Process Synthesis and Design 2</t>
+  </si>
+  <si>
+    <t>Unit Operations</t>
+  </si>
+  <si>
+    <t>Advanced Thermodynamics and Mass Transfer Processes</t>
+  </si>
+  <si>
+    <t>Reaction Engineering</t>
+  </si>
+  <si>
+    <t>Transport Phenomena</t>
+  </si>
+  <si>
+    <t>Advanced Reaction Engineering and Catalysts</t>
+  </si>
+  <si>
+    <t>Chemical Engineering Design Project</t>
+  </si>
+  <si>
+    <t>Chemical and Thermal Renewable Energies</t>
+  </si>
+  <si>
+    <t>Combustion Science and Technology</t>
+  </si>
+  <si>
+    <t>Flow Assurance for Future Energy</t>
+  </si>
+  <si>
+    <t>Gas Processing Technologies</t>
+  </si>
+  <si>
+    <t>Energy Storage Systems</t>
+  </si>
+  <si>
+    <t>Computational Data Analysis</t>
+  </si>
+  <si>
+    <t>Contaminant Fate and Transport</t>
+  </si>
+  <si>
+    <t>Extractive Metallurgy</t>
+  </si>
+  <si>
+    <t>Fossil to Future – The Transition</t>
+  </si>
+  <si>
+    <t>Modern Control Systems</t>
+  </si>
+  <si>
+    <t>Renewable Energy</t>
+  </si>
+  <si>
+    <t>GROUP_A_SP-ECHEM</t>
+  </si>
+  <si>
+    <t>GROUP_B_SP-ECHEM</t>
+  </si>
+  <si>
+    <t>CORE_SP-ESOFT</t>
   </si>
 </sst>
 </file>
@@ -300,12 +369,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -320,9 +395,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,24 +713,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDA6608-99D7-4958-A08E-79FB4C96684F}">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -688,19 +763,19 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
+      <c r="B2" t="s">
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -709,15 +784,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -726,15 +804,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -742,19 +823,19 @@
       <c r="G4">
         <v>6</v>
       </c>
-      <c r="K4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>18</v>
+      <c r="J4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -762,19 +843,19 @@
       <c r="G5">
         <v>6</v>
       </c>
-      <c r="K5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>21</v>
+      <c r="J5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -783,15 +864,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>19</v>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -799,19 +880,19 @@
       <c r="G7">
         <v>6</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>22</v>
+      <c r="J7" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -820,15 +901,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>23</v>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -837,15 +918,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>24</v>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -853,19 +934,22 @@
       <c r="G10">
         <v>6</v>
       </c>
-      <c r="L10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -873,19 +957,22 @@
       <c r="G11">
         <v>6</v>
       </c>
-      <c r="K11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>81</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -893,19 +980,22 @@
       <c r="G12">
         <v>6</v>
       </c>
-      <c r="K12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>82</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -913,19 +1003,19 @@
       <c r="G13">
         <v>6</v>
       </c>
-      <c r="K13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>28</v>
+      <c r="J13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -933,19 +1023,19 @@
       <c r="G14">
         <v>6</v>
       </c>
-      <c r="K14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>29</v>
+      <c r="J14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -954,15 +1044,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>30</v>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -970,19 +1060,22 @@
       <c r="G16">
         <v>6</v>
       </c>
-      <c r="K16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>83</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E17">
         <v>3</v>
@@ -990,22 +1083,25 @@
       <c r="G17">
         <v>6</v>
       </c>
+      <c r="J17" t="s">
+        <v>64</v>
+      </c>
       <c r="K17" t="s">
-        <v>68</v>
-      </c>
-      <c r="L17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>84</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E18">
         <v>3</v>
@@ -1013,19 +1109,22 @@
       <c r="G18">
         <v>6</v>
       </c>
-      <c r="K18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>85</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E19">
         <v>3</v>
@@ -1033,19 +1132,19 @@
       <c r="G19">
         <v>6</v>
       </c>
-      <c r="K19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>34</v>
+      <c r="J19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E20">
         <v>3</v>
@@ -1053,19 +1152,22 @@
       <c r="G20">
         <v>6</v>
       </c>
-      <c r="K20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>86</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E21">
         <v>3</v>
@@ -1073,19 +1175,22 @@
       <c r="G21">
         <v>6</v>
       </c>
-      <c r="K21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>87</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E22">
         <v>3</v>
@@ -1093,19 +1198,19 @@
       <c r="G22">
         <v>6</v>
       </c>
-      <c r="K22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>37</v>
+      <c r="J22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E23">
         <v>3</v>
@@ -1114,15 +1219,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>38</v>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E24">
         <v>3</v>
@@ -1130,19 +1235,19 @@
       <c r="G24">
         <v>6</v>
       </c>
-      <c r="K24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>39</v>
+      <c r="J24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E25">
         <v>5</v>
@@ -1150,25 +1255,28 @@
       <c r="G25">
         <v>0</v>
       </c>
-      <c r="I25">
+      <c r="H25">
         <v>144</v>
       </c>
-      <c r="J25" t="s">
-        <v>75</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I25" t="s">
+        <v>71</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E26">
         <v>4</v>
@@ -1176,19 +1284,22 @@
       <c r="G26">
         <v>6</v>
       </c>
-      <c r="K26" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
       </c>
       <c r="C27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E27">
         <v>5</v>
@@ -1196,19 +1307,19 @@
       <c r="G27">
         <v>12</v>
       </c>
-      <c r="K27" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>42</v>
+      <c r="J27" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E28">
         <v>4</v>
@@ -1216,19 +1327,19 @@
       <c r="G28">
         <v>6</v>
       </c>
-      <c r="I28">
+      <c r="H28">
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>43</v>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D29" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E29">
         <v>4</v>
@@ -1237,15 +1348,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>44</v>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D30" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="E30">
         <v>5</v>
@@ -1253,19 +1364,22 @@
       <c r="G30">
         <v>6</v>
       </c>
-      <c r="I30">
+      <c r="H30">
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="B31" t="s">
+        <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="E31">
         <v>4</v>
@@ -1273,19 +1387,22 @@
       <c r="G31">
         <v>6</v>
       </c>
-      <c r="I31">
+      <c r="H31">
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="B32" t="s">
+        <v>91</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D32" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="E32">
         <v>5</v>
@@ -1293,19 +1410,22 @@
       <c r="G32">
         <v>6</v>
       </c>
-      <c r="I32">
+      <c r="H32">
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="B33" t="s">
+        <v>92</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="E33">
         <v>5</v>
@@ -1313,19 +1433,22 @@
       <c r="G33">
         <v>6</v>
       </c>
-      <c r="I33">
+      <c r="H33">
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="B34" t="s">
+        <v>93</v>
       </c>
       <c r="C34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D34" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="E34">
         <v>5</v>
@@ -1333,19 +1456,22 @@
       <c r="G34">
         <v>6</v>
       </c>
-      <c r="I34">
+      <c r="H34">
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="B35" t="s">
+        <v>94</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="E35">
         <v>5</v>
@@ -1353,19 +1479,22 @@
       <c r="G35">
         <v>6</v>
       </c>
-      <c r="I35">
+      <c r="H35">
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="B36" t="s">
+        <v>95</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="E36">
         <v>4</v>
@@ -1373,19 +1502,22 @@
       <c r="G36">
         <v>6</v>
       </c>
-      <c r="I36">
+      <c r="H36">
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="B37" t="s">
+        <v>96</v>
       </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D37" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="E37">
         <v>4</v>
@@ -1393,19 +1525,22 @@
       <c r="G37">
         <v>6</v>
       </c>
-      <c r="I37">
+      <c r="H37">
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>51</v>
+      </c>
+      <c r="B38" t="s">
+        <v>97</v>
       </c>
       <c r="C38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="E38">
         <v>4</v>
@@ -1413,19 +1548,22 @@
       <c r="G38">
         <v>6</v>
       </c>
-      <c r="I38">
+      <c r="H38">
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>52</v>
+      </c>
+      <c r="B39" t="s">
+        <v>98</v>
       </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="E39">
         <v>4</v>
@@ -1433,19 +1571,22 @@
       <c r="G39">
         <v>6</v>
       </c>
-      <c r="I39">
+      <c r="H39">
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+      <c r="B40" t="s">
+        <v>99</v>
       </c>
       <c r="C40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="E40">
         <v>5</v>
@@ -1453,19 +1594,19 @@
       <c r="G40">
         <v>6</v>
       </c>
-      <c r="K40" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>58</v>
+      <c r="J40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="C41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D41" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="E41">
         <v>5</v>
@@ -1473,19 +1614,22 @@
       <c r="G41">
         <v>6</v>
       </c>
-      <c r="I41">
+      <c r="H41">
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>55</v>
+      </c>
+      <c r="B42" t="s">
+        <v>100</v>
       </c>
       <c r="C42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D42" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="E42">
         <v>5</v>
@@ -1493,11 +1637,11 @@
       <c r="G42">
         <v>6</v>
       </c>
-      <c r="I42">
+      <c r="H42">
         <v>120</v>
       </c>
-      <c r="K42" t="s">
-        <v>80</v>
+      <c r="J42" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>